<commit_message>
Saving work done so far
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zperkins/repos/nodejs_cysc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AFFE37-A04B-0A4C-A4D4-18A630C19FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 3" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet1" sheetId="2" r:id="rId5"/>
+    <sheet name="Form Responses 3" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_6EEBBF6C_B599_4331_948C_FD742946069E_.wvu.FilterData">'Form Responses 3'!$A$37</definedName>
+    <definedName name="Z_6EEBBF6C_B599_4331_948C_FD742946069E_.wvu.FilterData" localSheetId="0" hidden="1">'Form Responses 3'!$A$37</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{6EEBBF6C-B599-4331-948C-FD742946069E}" name="Filter 1"/>
+    <customWorkbookView name="Filter 1" guid="{6EEBBF6C-B599-4331-948C-FD742946069E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Timestamp</t>
   </si>
@@ -194,210 +203,140 @@
   </si>
   <si>
     <t>7:15</t>
-  </si>
-  <si>
-    <t>Performance Goals</t>
-  </si>
-  <si>
-    <t>Goal Running Pace</t>
-  </si>
-  <si>
-    <t>Goal Rucking Pace</t>
-  </si>
-  <si>
-    <t># Beatdowns</t>
-  </si>
-  <si>
-    <t># 5ks</t>
-  </si>
-  <si>
-    <t># 10ks</t>
-  </si>
-  <si>
-    <t># Halfs</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Fulls </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max # Burpees </t>
-  </si>
-  <si>
-    <t>Max # Merkins</t>
-  </si>
-  <si>
-    <t>Max # Big Boys</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="12.0"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9FC5E8"/>
-        <bgColor rgb="FF9FC5E8"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF8E3"/>
+          <bgColor rgb="FFFEF8E3"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF7CB4D"/>
           <bgColor rgb="FFF7CB4D"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF8E3"/>
-          <bgColor rgb="FFFEF8E3"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Form Responses 3-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Form Responses 3-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:U10" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:U10" headerRowCount="0">
   <tableColumns count="21">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
-    <tableColumn name="Column7" id="7"/>
-    <tableColumn name="Column8" id="8"/>
-    <tableColumn name="Column9" id="9"/>
-    <tableColumn name="Column10" id="10"/>
-    <tableColumn name="Column11" id="11"/>
-    <tableColumn name="Column12" id="12"/>
-    <tableColumn name="Column13" id="13"/>
-    <tableColumn name="Column14" id="14"/>
-    <tableColumn name="Column15" id="15"/>
-    <tableColumn name="Column16" id="16"/>
-    <tableColumn name="Column17" id="17"/>
-    <tableColumn name="Column18" id="18"/>
-    <tableColumn name="Column19" id="19"/>
-    <tableColumn name="Column20" id="20"/>
-    <tableColumn name="Column21" id="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21"/>
   </tableColumns>
-  <tableStyleInfo name="Form Responses 3-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Form Responses 3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
@@ -407,7 +346,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -597,26 +536,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="21" width="21.57"/>
+    <col min="1" max="21" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,11 +611,11 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>44553.376027962964</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -692,28 +634,28 @@
         <v>9.9</v>
       </c>
       <c r="H2" s="3">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="I2" s="3">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="J2" s="3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="K2" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N2" s="3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="O2" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -722,9 +664,9 @@
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <v>44552.98093546296</v>
+        <v>44552.980935462961</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>20</v>
@@ -742,27 +684,27 @@
         <v>24</v>
       </c>
       <c r="G3" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="I3" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="N3" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="O3" s="3">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -771,9 +713,9 @@
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <v>44552.69537990741</v>
+        <v>44552.695379907411</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>25</v>
@@ -791,29 +733,29 @@
         <v>29</v>
       </c>
       <c r="G4" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="3">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="I4" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="J4" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="K4" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="3">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="N4" s="3">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="O4" s="3">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
@@ -822,7 +764,7 @@
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>44553.363860763886</v>
       </c>
@@ -842,31 +784,31 @@
         <v>34</v>
       </c>
       <c r="G5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="3">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="I5" s="3">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="J5" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="K5" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="3">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="N5" s="3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="O5" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -875,7 +817,7 @@
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6">
         <v>44553.469819872684</v>
       </c>
@@ -895,19 +837,19 @@
         <v>39</v>
       </c>
       <c r="I6" s="7">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J6" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M6" s="7">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="N6" s="7">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="O6" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -916,9 +858,9 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>44553.38391421296</v>
+        <v>44553.383914212958</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>40</v>
@@ -936,31 +878,31 @@
         <v>19</v>
       </c>
       <c r="G7" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H7" s="3">
-        <v>208.0</v>
+        <v>208</v>
       </c>
       <c r="I7" s="3">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="J7" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="K7" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="3">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="N7" s="3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="O7" s="3">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -969,9 +911,9 @@
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6">
-        <v>44553.51212047454</v>
+        <v>44553.512120474537</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>44</v>
@@ -992,30 +934,30 @@
         <v>3.5</v>
       </c>
       <c r="H8" s="7">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="I8" s="7">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="J8" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K8" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M8" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N8" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="O8" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6">
-        <v>44553.7113078588</v>
+        <v>44553.711307858801</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>49</v>
@@ -1033,30 +975,30 @@
         <v>53</v>
       </c>
       <c r="H9" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="I9" s="7">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="J9" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K9" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="7">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="N9" s="7">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="O9" s="7">
-        <v>50.0</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
-        <v>44553.79877440972</v>
+        <v>44553.798774409719</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>54</v>
@@ -1074,112 +1016,40 @@
         <v>58</v>
       </c>
       <c r="H10" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="I10" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J10" s="7">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="K10" s="7">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="M10" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N10" s="7">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="O10" s="7">
-        <v>150.0</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6EEBBF6C-B599-4331-948C-FD742946069E}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$A$37"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A37" xr:uid="{56B9BEB5-45F1-0141-A503-F90D2A3FDECC}"/>
     </customSheetView>
   </customSheetViews>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A9CCB529-DCCD-AF48-89C5-7723777C9A89}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="22.57"/>
-    <col customWidth="1" min="2" max="2" width="19.57"/>
-    <col customWidth="1" min="3" max="3" width="20.71"/>
-    <col customWidth="1" min="4" max="4" width="21.0"/>
-    <col customWidth="1" min="5" max="5" width="18.86"/>
-    <col customWidth="1" min="6" max="6" width="18.57"/>
-    <col customWidth="1" min="7" max="7" width="17.0"/>
-    <col customWidth="1" min="8" max="8" width="17.71"/>
-    <col customWidth="1" min="9" max="9" width="18.71"/>
-    <col customWidth="1" min="10" max="10" width="17.14"/>
-    <col customWidth="1" min="11" max="11" width="17.43"/>
-    <col customWidth="1" min="12" max="12" width="19.14"/>
-    <col customWidth="1" min="13" max="13" width="21.57"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>